<commit_message>
bsdata bucketing commit 2 mar afternoon
</commit_message>
<xml_diff>
--- a/output/599060e9-8b46-46ec-87b9-c79cde8a82b7/599060e9-8b46-46ec-87b9-c79cde8a82b7_notes_cropped_df.xlsx
+++ b/output/599060e9-8b46-46ec-87b9-c79cde8a82b7/599060e9-8b46-46ec-87b9-c79cde8a82b7_notes_cropped_df.xlsx
@@ -7,26 +7,83 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="783d1f36-c06c-3414-a" sheetId="1" r:id="rId1"/>
-    <sheet name="6354e3c7-4619-3a07-b" sheetId="2" r:id="rId2"/>
-    <sheet name="09af3f09-68b9-3555-9" sheetId="3" r:id="rId3"/>
-    <sheet name="e3601430-2dd6-3395-9" sheetId="4" r:id="rId4"/>
-    <sheet name="bb79b34d-1e9c-34e4-a" sheetId="5" r:id="rId5"/>
-    <sheet name="24662bf7-9672-32e9-9" sheetId="6" r:id="rId6"/>
-    <sheet name="2307c038-33fd-3bed-8" sheetId="7" r:id="rId7"/>
-    <sheet name="6bafd8f6-8a94-32ee-9" sheetId="8" r:id="rId8"/>
-    <sheet name="65990df0-8285-3b32-8" sheetId="9" r:id="rId9"/>
-    <sheet name="8a5d8593-402f-3237-9" sheetId="10" r:id="rId10"/>
-    <sheet name="85574d29-1138-3d46-a" sheetId="11" r:id="rId11"/>
-    <sheet name="e8b583fe-7a0d-3304-9" sheetId="12" r:id="rId12"/>
-    <sheet name="dfb38738-8ae6-3592-8" sheetId="13" r:id="rId13"/>
+    <sheet name="6__783d1f36-c06c-341" sheetId="1" r:id="rId1"/>
+    <sheet name="7__783d1f36-c06c-341" sheetId="2" r:id="rId2"/>
+    <sheet name="8__783d1f36-c06c-341" sheetId="3" r:id="rId3"/>
+    <sheet name="9__6354e3c7-4619-3a0" sheetId="4" r:id="rId4"/>
+    <sheet name="11__09af3f09-68b9-35" sheetId="5" r:id="rId5"/>
+    <sheet name="11__e3601430-2dd6-33" sheetId="6" r:id="rId6"/>
+    <sheet name="11__bb79b34d-1e9c-34" sheetId="7" r:id="rId7"/>
+    <sheet name="12__24662bf7-9672-32" sheetId="8" r:id="rId8"/>
+    <sheet name="16__2307c038-33fd-3b" sheetId="9" r:id="rId9"/>
+    <sheet name="16__6bafd8f6-8a94-32" sheetId="10" r:id="rId10"/>
+    <sheet name="17__65990df0-8285-3b" sheetId="11" r:id="rId11"/>
+    <sheet name="15__2307c038-33fd-3b" sheetId="12" r:id="rId12"/>
+    <sheet name="18__8a5d8593-402f-32" sheetId="13" r:id="rId13"/>
+    <sheet name="19__85574d29-1138-3d" sheetId="14" r:id="rId14"/>
+    <sheet name="4_1_e8b583fe-7a0d-33" sheetId="15" r:id="rId15"/>
+    <sheet name="4_2_e8b583fe-7a0d-33" sheetId="16" r:id="rId16"/>
+    <sheet name="4_3_e8b583fe-7a0d-33" sheetId="17" r:id="rId17"/>
+    <sheet name="4_4_dfb38738-8ae6-35" sheetId="18" r:id="rId18"/>
+    <sheet name="4_5_dfb38738-8ae6-35" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="248">
+  <si>
+    <t>6. Cash and cash equivalents</t>
+  </si>
+  <si>
+    <t>Cash at bank and on hand</t>
+  </si>
+  <si>
+    <t>Cash at banks earns interest at floating rates based on daily bank deposit rates.</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>$000</t>
+  </si>
+  <si>
+    <t>19589</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>28259</t>
+  </si>
+  <si>
+    <t>Trade and other receivables</t>
+  </si>
+  <si>
+    <t>GST receivable</t>
+  </si>
+  <si>
+    <t>Related party receivables (Note 20)</t>
+  </si>
+  <si>
+    <t>1697</t>
+  </si>
+  <si>
+    <t>11927</t>
+  </si>
+  <si>
+    <t>13624</t>
+  </si>
+  <si>
+    <t>1390</t>
+  </si>
+  <si>
+    <t>10609</t>
+  </si>
+  <si>
+    <t>11999</t>
+  </si>
   <si>
     <t>8. Inventories</t>
   </si>
@@ -37,12 +94,6 @@
     <t>Finished goods</t>
   </si>
   <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>$000</t>
-  </si>
-  <si>
     <t>18547</t>
   </si>
   <si>
@@ -52,9 +103,6 @@
     <t>27198</t>
   </si>
   <si>
-    <t>2019</t>
-  </si>
-  <si>
     <t>19816</t>
   </si>
   <si>
@@ -346,6 +394,156 @@
     <t>3731</t>
   </si>
   <si>
+    <t>16. Borrowings</t>
+  </si>
+  <si>
+    <t>Bank borrowings</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>facilities</t>
+  </si>
+  <si>
+    <t>Utilised</t>
+  </si>
+  <si>
+    <t>Balance at 31 December</t>
+  </si>
+  <si>
+    <t>bank guarantees</t>
+  </si>
+  <si>
+    <t>Multi-option facilities</t>
+  </si>
+  <si>
+    <t>52100</t>
+  </si>
+  <si>
+    <t>3273</t>
+  </si>
+  <si>
+    <t>48827</t>
+  </si>
+  <si>
+    <t>Bank guarantee facilities</t>
+  </si>
+  <si>
+    <t>13500</t>
+  </si>
+  <si>
+    <t>1023</t>
+  </si>
+  <si>
+    <t>47077</t>
+  </si>
+  <si>
+    <t>Arising during the year</t>
+  </si>
+  <si>
+    <t>Unwinding of discount</t>
+  </si>
+  <si>
+    <t>At31 December 2020</t>
+  </si>
+  <si>
+    <t>Employee benefits</t>
+  </si>
+  <si>
+    <t>4343</t>
+  </si>
+  <si>
+    <t>541</t>
+  </si>
+  <si>
+    <t>4884</t>
+  </si>
+  <si>
+    <t>4846</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>Workers compensation</t>
+  </si>
+  <si>
+    <t>3725</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>3884</t>
+  </si>
+  <si>
+    <t>Defined Benefit</t>
+  </si>
+  <si>
+    <t>865</t>
+  </si>
+  <si>
+    <t>(518)</t>
+  </si>
+  <si>
+    <t>347</t>
+  </si>
+  <si>
+    <t>Provision for asset retirement obligation</t>
+  </si>
+  <si>
+    <t>4806</t>
+  </si>
+  <si>
+    <t>36032</t>
+  </si>
+  <si>
+    <t>(336)</t>
+  </si>
+  <si>
+    <t>40502</t>
+  </si>
+  <si>
+    <t>Provision for carbon dust and other</t>
+  </si>
+  <si>
+    <t>6983</t>
+  </si>
+  <si>
+    <t>1286</t>
+  </si>
+  <si>
+    <t>8269</t>
+  </si>
+  <si>
+    <t>729</t>
+  </si>
+  <si>
+    <t>7540</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>19857</t>
+  </si>
+  <si>
+    <t>38883</t>
+  </si>
+  <si>
+    <t>(854)</t>
+  </si>
+  <si>
+    <t>57886</t>
+  </si>
+  <si>
+    <t>9459</t>
+  </si>
+  <si>
+    <t>48427</t>
+  </si>
+  <si>
     <t>15. Financial liabilities</t>
   </si>
   <si>
@@ -376,150 +574,6 @@
     <t>3895</t>
   </si>
   <si>
-    <t>facilities</t>
-  </si>
-  <si>
-    <t>Utilised</t>
-  </si>
-  <si>
-    <t>Balance at 31 December</t>
-  </si>
-  <si>
-    <t>bank guarantees</t>
-  </si>
-  <si>
-    <t>Multi-option facilities</t>
-  </si>
-  <si>
-    <t>52100</t>
-  </si>
-  <si>
-    <t>3273</t>
-  </si>
-  <si>
-    <t>48827</t>
-  </si>
-  <si>
-    <t>Bank guarantee facilities</t>
-  </si>
-  <si>
-    <t>13500</t>
-  </si>
-  <si>
-    <t>4000</t>
-  </si>
-  <si>
-    <t>1023</t>
-  </si>
-  <si>
-    <t>47077</t>
-  </si>
-  <si>
-    <t>Arising during the year</t>
-  </si>
-  <si>
-    <t>Unwinding of discount</t>
-  </si>
-  <si>
-    <t>At31 December 2020</t>
-  </si>
-  <si>
-    <t>Employee benefits</t>
-  </si>
-  <si>
-    <t>4343</t>
-  </si>
-  <si>
-    <t>541</t>
-  </si>
-  <si>
-    <t>4884</t>
-  </si>
-  <si>
-    <t>4846</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>Workers compensation</t>
-  </si>
-  <si>
-    <t>3725</t>
-  </si>
-  <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>3884</t>
-  </si>
-  <si>
-    <t>Defined Benefit</t>
-  </si>
-  <si>
-    <t>865</t>
-  </si>
-  <si>
-    <t>(518)</t>
-  </si>
-  <si>
-    <t>347</t>
-  </si>
-  <si>
-    <t>Provision for asset retirement obligation</t>
-  </si>
-  <si>
-    <t>4806</t>
-  </si>
-  <si>
-    <t>36032</t>
-  </si>
-  <si>
-    <t>(336)</t>
-  </si>
-  <si>
-    <t>40502</t>
-  </si>
-  <si>
-    <t>Provision for carbon dust and other</t>
-  </si>
-  <si>
-    <t>6983</t>
-  </si>
-  <si>
-    <t>1286</t>
-  </si>
-  <si>
-    <t>8269</t>
-  </si>
-  <si>
-    <t>729</t>
-  </si>
-  <si>
-    <t>7540</t>
-  </si>
-  <si>
-    <t>Totals</t>
-  </si>
-  <si>
-    <t>19857</t>
-  </si>
-  <si>
-    <t>38883</t>
-  </si>
-  <si>
-    <t>(854)</t>
-  </si>
-  <si>
-    <t>57886</t>
-  </si>
-  <si>
-    <t>9459</t>
-  </si>
-  <si>
-    <t>48427</t>
-  </si>
-  <si>
     <t>155,299,534 ordinary shares issued and fully paid (2019: 155,299,534)</t>
   </si>
   <si>
@@ -589,6 +643,69 @@
     <t>(9,032)</t>
   </si>
   <si>
+    <t>4.1 Revenue from contracts with customers</t>
+  </si>
+  <si>
+    <t>Disaggregated revenue information</t>
+  </si>
+  <si>
+    <t>Set out below is the disaggregation of the Company's revenue from contracts with customers:</t>
+  </si>
+  <si>
+    <t>Type of goods</t>
+  </si>
+  <si>
+    <t>Sale of goods</t>
+  </si>
+  <si>
+    <t>Total revenue from contracts with customers</t>
+  </si>
+  <si>
+    <t>Geographical markets</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Timing of revenue recognition</t>
+  </si>
+  <si>
+    <t>Goods transferred at a point in time</t>
+  </si>
+  <si>
+    <t>214911</t>
+  </si>
+  <si>
+    <t>190814</t>
+  </si>
+  <si>
+    <t>24097</t>
+  </si>
+  <si>
+    <t>229785</t>
+  </si>
+  <si>
+    <t>197789</t>
+  </si>
+  <si>
+    <t>31996</t>
+  </si>
+  <si>
+    <t>4.2 Other revenue</t>
+  </si>
+  <si>
+    <t>Commission revenue</t>
+  </si>
+  <si>
+    <t>775</t>
+  </si>
+  <si>
+    <t>780</t>
+  </si>
+  <si>
     <t>4.3 Other income</t>
   </si>
   <si>
@@ -626,6 +743,15 @@
   </si>
   <si>
     <t>10144</t>
+  </si>
+  <si>
+    <t>Bank interest</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>170</t>
   </si>
   <si>
     <t>4.5 Finance costs</t>
@@ -1007,7 +1133,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1037,7 +1163,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1056,26 +1182,15 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
+      <c r="B6" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1084,6 +1199,394 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1107,7 +1610,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1120,13 +1623,13 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -1155,7 +1658,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1163,7 +1666,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1176,40 +1679,40 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1217,7 +1720,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1230,40 +1733,40 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B12" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1271,7 +1774,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1284,29 +1787,29 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1314,7 +1817,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1327,40 +1830,40 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="C23" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="C25" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1368,7 +1871,210 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1389,7 +2095,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1397,7 +2103,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1410,48 +2116,48 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>225</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>229</v>
       </c>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>227</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>230</v>
       </c>
       <c r="C8" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="B9" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="C9" t="s">
-        <v>199</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -1459,7 +2165,58 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1480,7 +2237,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1488,7 +2245,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1501,32 +2258,32 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>243</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>204</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>207</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -1535,6 +2292,162 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -1555,7 +2468,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1563,7 +2476,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1576,41 +2489,41 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="C8" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1618,7 +2531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -1648,16 +2561,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="C2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1665,27 +2578,27 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -1696,27 +2609,27 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1724,7 +2637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -1751,7 +2664,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1764,46 +2677,46 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1811,7 +2724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1832,7 +2745,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1840,7 +2753,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1853,13 +2766,13 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1867,7 +2780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -1897,24 +2810,24 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1936,224 +2849,224 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="F8" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F18" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2161,9 +3074,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2182,366 +3095,31 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="C8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="C3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" t="s">
         <v>122</v>
-      </c>
-      <c r="D7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" t="s">
-        <v>149</v>
-      </c>
-      <c r="G5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F6" t="s">
-        <v>154</v>
-      </c>
-      <c r="G6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F7" t="s">
-        <v>155</v>
-      </c>
-      <c r="G7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" t="s">
-        <v>150</v>
-      </c>
-      <c r="F8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G8" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>